<commit_message>
Updated CF - Create Email Campaign					Updates - Syndication Status API,LPAD and DTC					Updated - Duplicate Management
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{73D8C436-39E3-48C9-B63A-60500FBB6AB2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B2C74A8D-01A7-41A1-94BF-6BA03064978A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateCampaign" r:id="rId1" sheetId="1"/>
+    <sheet name="EmailLocationCampaign" r:id="rId1" sheetId="1"/>
     <sheet name="Date" r:id="rId2" sheetId="2"/>
+    <sheet name="Reschedule Date" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>CamType</t>
   </si>
@@ -40,7 +41,7 @@
     <t>CamName</t>
   </si>
   <si>
-    <t>CamDesc</t>
+    <t>CamDes</t>
   </si>
   <si>
     <t>Location</t>
@@ -73,7 +74,10 @@
     <t>Campaign Test</t>
   </si>
   <si>
-    <t>Campaign Desc Test</t>
+    <t xml:space="preserve">Test </t>
+  </si>
+  <si>
+    <t>Alexis Multispeciality Hospital</t>
   </si>
   <si>
     <t>amahadev@dacgroup.com</t>
@@ -82,59 +86,92 @@
     <t>Avinash</t>
   </si>
   <si>
-    <t>Campaign Schedule</t>
-  </si>
-  <si>
-    <t>Campaign Details</t>
-  </si>
-  <si>
-    <t>Hi, Please Test</t>
-  </si>
-  <si>
-    <t>Thanks and Regards,
+    <t>Campaign FeedBack</t>
+  </si>
+  <si>
+    <t>Please provide feedback</t>
+  </si>
+  <si>
+    <t>Please feel free to share your experience</t>
+  </si>
+  <si>
+    <t>Thanks and Regards
 Avinash</t>
   </si>
   <si>
+    <t>1Star Messaging</t>
+  </si>
+  <si>
+    <t>3Star Messaging</t>
+  </si>
+  <si>
+    <t>4Star Messaging</t>
+  </si>
+  <si>
+    <t>Thanks you for feedback</t>
+  </si>
+  <si>
+    <t>Thanks for your feedback! Have a greatday</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>I had a poor experience</t>
+  </si>
+  <si>
+    <t>ReSchedule CampName</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>Day_DD</t>
+  </si>
+  <si>
+    <t>Month_MMM</t>
+  </si>
+  <si>
+    <t>Year_YYYY</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
     <t>Time</t>
   </si>
   <si>
-    <t>FromDate</t>
-  </si>
-  <si>
-    <t>ToDate</t>
-  </si>
-  <si>
-    <t>Day_DD</t>
-  </si>
-  <si>
-    <t>Month_MMM</t>
-  </si>
-  <si>
-    <t>Year_YYYY</t>
-  </si>
-  <si>
-    <t>08:00 PM</t>
-  </si>
-  <si>
-    <t>1Star Messaging</t>
-  </si>
-  <si>
-    <t>3Star Messaging</t>
-  </si>
-  <si>
-    <t>4Star Messaging</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>Alexis Multispeciality Hospital</t>
-  </si>
-  <si>
-    <t>May</t>
+    <t>10:00 PM</t>
   </si>
   <si>
     <t>June</t>
+  </si>
+  <si>
+    <t>Campaign Test06/03/2020 9:22:35 PM</t>
+  </si>
+  <si>
+    <t>Sorry for your experience and we'll make sure you will have better experience next time</t>
+  </si>
+  <si>
+    <t>Campaign Test06/03/2020 9:32:09 PM</t>
+  </si>
+  <si>
+    <t>Campaign Test06/03/2020 9:38:52 PM</t>
   </si>
 </sst>
 </file>
@@ -142,16 +179,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -186,18 +215,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -481,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,66 +519,81 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="134.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="13" max="15" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>31</v>
+      <c r="S1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row ht="45" r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -568,117 +610,198 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="R2" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
+      <c r="S2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2" xr:uid="{8073A71E-16DA-492C-8655-1487631AC4CE}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3418EE62-AF27-45C6-BFA4-3A437CC26903}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>28</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D3" s="3">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="4">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3">
         <v>2020</v>
       </c>
-      <c r="D3" s="4">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="D3" s="3">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3">
         <v>2020</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Email Campaign - CF
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{B2C74A8D-01A7-41A1-94BF-6BA03064978A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E040C1C6-CDF7-4B69-8885-6FCB0FBFC771}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="EmailLocationCampaign" r:id="rId1" sheetId="1"/>
     <sheet name="Date" r:id="rId2" sheetId="2"/>
     <sheet name="Reschedule Date" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>CamType</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Year_YYYY</t>
   </si>
   <si>
-    <t>July</t>
-  </si>
-  <si>
     <t>August</t>
   </si>
   <si>
@@ -159,19 +157,22 @@
     <t>10:00 PM</t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>Campaign Test06/03/2020 9:22:35 PM</t>
-  </si>
-  <si>
     <t>Sorry for your experience and we'll make sure you will have better experience next time</t>
   </si>
   <si>
-    <t>Campaign Test06/03/2020 9:32:09 PM</t>
-  </si>
-  <si>
-    <t>Campaign Test06/03/2020 9:38:52 PM</t>
+    <t>NTBACF02</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>Campaign Test06/12/2020 4:01:43 PM</t>
+  </si>
+  <si>
+    <t>Campaign Test06/12/2020 5:03:38 PM</t>
+  </si>
+  <si>
+    <t>Campaign Test06/12/2020 5:25:10 PM</t>
   </si>
 </sst>
 </file>
@@ -510,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +611,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -631,7 +632,7 @@
         <v>22</v>
       </c>
       <c r="M2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
         <v>26</v>
@@ -657,6 +658,7 @@
     <hyperlink r:id="rId1" ref="G2" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -682,7 +684,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -705,7 +707,7 @@
         <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -713,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3">
         <v>2020</v>
@@ -722,7 +724,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3">
         <v>2020</v>
@@ -741,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +761,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -782,7 +784,7 @@
         <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -796,10 +798,10 @@
         <v>2020</v>
       </c>
       <c r="D3" s="3">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3">
         <v>2020</v>
@@ -812,4 +814,22 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Files of CF
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{E040C1C6-CDF7-4B69-8885-6FCB0FBFC771}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0CA264-BDD4-457E-8530-556C842BC4F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EmailLocationCampaign" r:id="rId1" sheetId="1"/>
-    <sheet name="Date" r:id="rId2" sheetId="2"/>
-    <sheet name="Reschedule Date" r:id="rId3" sheetId="3"/>
-    <sheet name="Sheet1" r:id="rId4" sheetId="4"/>
+    <sheet name="EmailLocationCampaign" sheetId="1" r:id="rId1"/>
+    <sheet name="EmailBrandCampaign" sheetId="6" r:id="rId2"/>
+    <sheet name="GRLocationCampaign" sheetId="5" r:id="rId3"/>
+    <sheet name="Date" sheetId="2" r:id="rId4"/>
+    <sheet name="Reschedule Date" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>CamType</t>
   </si>
@@ -166,21 +168,59 @@
     <t>September</t>
   </si>
   <si>
-    <t>Campaign Test06/12/2020 4:01:43 PM</t>
-  </si>
-  <si>
-    <t>Campaign Test06/12/2020 5:03:38 PM</t>
-  </si>
-  <si>
-    <t>Campaign Test06/12/2020 5:25:10 PM</t>
+    <t>Brand Name</t>
+  </si>
+  <si>
+    <t>Address Line</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Postal</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Auto Test</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Trivandrum</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>658881</t>
+  </si>
+  <si>
+    <t>9098674532</t>
+  </si>
+  <si>
+    <t>Campaign Test06/15/2020 8:33:17 PM</t>
+  </si>
+  <si>
+    <t>General R Location</t>
+  </si>
+  <si>
+    <t>General Review Link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +232,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,26 +263,35 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -251,10 +308,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -289,7 +346,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -324,7 +381,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -418,21 +475,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -449,7 +506,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -501,38 +558,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="79" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -594,7 +651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row ht="45" r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -650,21 +707,297 @@
         <v>32</v>
       </c>
       <c r="S2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180802A0-94AE-4CA7-8363-1BACCC04771F}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="38.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="81.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="39.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="34.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="16384" width="9.140625" style="2" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{EFD0683B-08D1-422F-95F9-F3247753FAE0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -673,16 +1006,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" t="s">
         <v>40</v>
       </c>
@@ -735,31 +1068,31 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
-  <dimension ref="A1:H3"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
       <c r="G1" t="s">
         <v>40</v>
       </c>
@@ -812,13 +1145,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
-  <dimension ref="A1:B1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -830,6 +1163,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated GRL_Location campaign code
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0CA264-BDD4-457E-8530-556C842BC4F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214E3E2F-095A-4DFF-A286-E55492142BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>CamType</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>General Review Link</t>
+  </si>
+  <si>
+    <t>ProcessedCampaign Name</t>
   </si>
 </sst>
 </file>
@@ -913,10 +916,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,9 +933,10 @@
     <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,8 +964,11 @@
       <c r="I1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Updated code for General Review Link with Location create campaign CF
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214E3E2F-095A-4DFF-A286-E55492142BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C88F8AB-706F-446B-A60D-4C9547D7654B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmailLocationCampaign" sheetId="1" r:id="rId1"/>
     <sheet name="EmailBrandCampaign" sheetId="6" r:id="rId2"/>
     <sheet name="GRLocationCampaign" sheetId="5" r:id="rId3"/>
-    <sheet name="Date" sheetId="2" r:id="rId4"/>
-    <sheet name="Reschedule Date" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId6"/>
+    <sheet name="GRLBrandCampaign" sheetId="7" r:id="rId4"/>
+    <sheet name="Date" sheetId="2" r:id="rId5"/>
+    <sheet name="Reschedule Date" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
   <si>
     <t>CamType</t>
   </si>
@@ -217,6 +218,21 @@
   </si>
   <si>
     <t>ProcessedCampaign Name</t>
+  </si>
+  <si>
+    <t>Address Line1</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>685098</t>
+  </si>
+  <si>
+    <t>9900985634</t>
   </si>
 </sst>
 </file>
@@ -269,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -288,6 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,7 +589,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:S2"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,6 +1020,128 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62030C4F-85F5-4D7C-AEBE-444ECD7E4204}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="81.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1079,7 +1218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1156,7 +1295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated Create Campaign Scenarios for CF
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C88F8AB-706F-446B-A60D-4C9547D7654B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CEAD50B2-6B03-44A3-AA87-C676CCEA362F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="EmailLocationCampaign" sheetId="1" r:id="rId1"/>
-    <sheet name="EmailBrandCampaign" sheetId="6" r:id="rId2"/>
-    <sheet name="GRLocationCampaign" sheetId="5" r:id="rId3"/>
-    <sheet name="GRLBrandCampaign" sheetId="7" r:id="rId4"/>
-    <sheet name="Date" sheetId="2" r:id="rId5"/>
-    <sheet name="Reschedule Date" sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId7"/>
+    <sheet name="EmailLocationCampaign" r:id="rId1" sheetId="1"/>
+    <sheet name="EmailBrandCampaign" r:id="rId2" sheetId="6"/>
+    <sheet name="EmailMultiLocation" r:id="rId3" sheetId="8"/>
+    <sheet name="GRLocationCampaign" r:id="rId4" sheetId="5"/>
+    <sheet name="GRLBrandCampaign" r:id="rId5" sheetId="7"/>
+    <sheet name="Date" r:id="rId6" sheetId="2"/>
+    <sheet name="Reschedule Date" r:id="rId7" sheetId="3"/>
+    <sheet name="Sheet1" r:id="rId8" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="75">
   <si>
     <t>CamType</t>
   </si>
@@ -233,12 +234,37 @@
   </si>
   <si>
     <t>9900985634</t>
+  </si>
+  <si>
+    <t>General R Location06/19/2020 7:25:42 AM</t>
+  </si>
+  <si>
+    <t>Multi-location</t>
+  </si>
+  <si>
+    <t>MultiLocation Test</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>9000334772,9000334773,9000334774</t>
+  </si>
+  <si>
+    <t>MultiLocation Test06/24/2020 10:48:53 AM</t>
+  </si>
+  <si>
+    <t>MultiLocation Test06/24/2020 10:58:38 AM</t>
+  </si>
+  <si>
+    <t>MultiLocation Test06/24/2020 11:06:56 AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -282,36 +308,36 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -328,10 +354,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -366,7 +392,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -401,7 +427,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -495,21 +521,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -526,7 +552,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -578,15 +604,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
@@ -594,22 +620,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="79" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -671,7 +697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -732,51 +758,51 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180802A0-94AE-4CA7-8363-1BACCC04771F}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180802A0-94AE-4CA7-8363-1BACCC04771F}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="38.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="81.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="39.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="34.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="23.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="38.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="14.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="81.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="34.28515625" collapsed="true"/>
+    <col min="25" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -850,7 +876,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -924,33 +950,161 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{EFD0683B-08D1-422F-95F9-F3247753FAE0}"/>
+    <hyperlink r:id="rId1" ref="L2" xr:uid="{EFD0683B-08D1-422F-95F9-F3247753FAE0}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B2BB62-79BB-4A73-9996-95362A466A26}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="32.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="81.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="23.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="38.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="27.0" collapsed="true"/>
+    <col min="16" max="16384" style="2" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row ht="30" r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row ht="30" r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1015,79 +1169,79 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62030C4F-85F5-4D7C-AEBE-444ECD7E4204}">
-  <dimension ref="A1:O2"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62030C4F-85F5-4D7C-AEBE-444ECD7E4204}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="81.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="8" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1134,16 +1288,19 @@
       <c r="N2" t="s">
         <v>27</v>
       </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1152,16 +1309,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" t="s">
         <v>40</v>
       </c>
@@ -1214,13 +1371,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -1229,16 +1386,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" t="s">
         <v>40</v>
       </c>
@@ -1291,13 +1448,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1309,6 +1466,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated TSEE and CF - Filter Verification
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{CEAD50B2-6B03-44A3-AA87-C676CCEA362F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E61F17-5C48-4FE1-9751-59291F71512F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EmailLocationCampaign" r:id="rId1" sheetId="1"/>
-    <sheet name="EmailBrandCampaign" r:id="rId2" sheetId="6"/>
-    <sheet name="EmailMultiLocation" r:id="rId3" sheetId="8"/>
-    <sheet name="GRLocationCampaign" r:id="rId4" sheetId="5"/>
-    <sheet name="GRLBrandCampaign" r:id="rId5" sheetId="7"/>
-    <sheet name="Date" r:id="rId6" sheetId="2"/>
-    <sheet name="Reschedule Date" r:id="rId7" sheetId="3"/>
-    <sheet name="Sheet1" r:id="rId8" sheetId="4"/>
+    <sheet name="EmailLocationCampaign" sheetId="1" r:id="rId1"/>
+    <sheet name="EmailBrandCampaign" sheetId="6" r:id="rId2"/>
+    <sheet name="EmailMultiLocation" sheetId="8" r:id="rId3"/>
+    <sheet name="GRLocationCampaign" sheetId="5" r:id="rId4"/>
+    <sheet name="GRLBrandCampaign" sheetId="7" r:id="rId5"/>
+    <sheet name="GRLMultiLocation" sheetId="9" r:id="rId6"/>
+    <sheet name="Date" sheetId="2" r:id="rId7"/>
+    <sheet name="Reschedule Date" sheetId="3" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId9"/>
+    <sheet name="Filters" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="78">
   <si>
     <t>CamType</t>
   </si>
@@ -251,20 +253,28 @@
     <t>9000334772,9000334773,9000334774</t>
   </si>
   <si>
-    <t>MultiLocation Test06/24/2020 10:48:53 AM</t>
-  </si>
-  <si>
-    <t>MultiLocation Test06/24/2020 10:58:38 AM</t>
-  </si>
-  <si>
-    <t>MultiLocation Test06/24/2020 11:06:56 AM</t>
+    <t>GRL MultiLocation Test</t>
+  </si>
+  <si>
+    <t>MultiLocation Test06/25/2020 7:05:30 AM</t>
+  </si>
+  <si>
+    <t>GRL MultiLocation Test06/25/2020 8:05:25 AM</t>
+  </si>
+  <si>
+    <t>FilterType</t>
+  </si>
+  <si>
+    <t>FilterSetUp</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -308,36 +318,39 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -354,10 +367,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -392,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -427,7 +440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -521,21 +534,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -552,7 +565,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -604,15 +617,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
@@ -620,22 +633,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="79" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -697,7 +710,7 @@
         <v>33</v>
       </c>
     </row>
-    <row ht="45" r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -758,16 +771,75 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7CE0A5-DECB-4987-BD51-DB8EFDE59B69}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180802A0-94AE-4CA7-8363-1BACCC04771F}">
-  <dimension ref="A1:Y2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180802A0-94AE-4CA7-8363-1BACCC04771F}">
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:Q2"/>
@@ -775,34 +847,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="8.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="23.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="38.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="14.85546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="81.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="34.28515625" collapsed="true"/>
-    <col min="25" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="38.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="81.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="39.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="34.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -876,7 +948,7 @@
         <v>33</v>
       </c>
     </row>
-    <row ht="45" r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -950,42 +1022,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="L2" xr:uid="{EFD0683B-08D1-422F-95F9-F3247753FAE0}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{EFD0683B-08D1-422F-95F9-F3247753FAE0}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B2BB62-79BB-4A73-9996-95362A466A26}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B2BB62-79BB-4A73-9996-95362A466A26}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="8.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="32.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="81.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="23.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="38.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="27.0" collapsed="true"/>
-    <col min="16" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="81.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="39.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="38.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1061,7 +1133,7 @@
         <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>18</v>
@@ -1080,14 +1152,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:I2"/>
@@ -1095,16 +1167,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1169,33 +1241,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62030C4F-85F5-4D7C-AEBE-444ECD7E4204}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62030C4F-85F5-4D7C-AEBE-444ECD7E4204}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="8" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1293,14 +1363,105 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F67BC90-6774-475B-9753-7D297B7B4830}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1309,16 +1470,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" t="s">
         <v>40</v>
       </c>
@@ -1371,13 +1532,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
-  <dimension ref="A1:H3"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -1386,16 +1547,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
       <c r="G1" t="s">
         <v>40</v>
       </c>
@@ -1448,13 +1609,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
-  <dimension ref="A1:B1"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1466,6 +1627,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1)Updated Number of entries method					2)Updated CF Test Data file					3)Updated Campaigns Page for Filters					4)Created and Updated Verify Filters Test class
</commit_message>
<xml_diff>
--- a/data/CF.xlsx
+++ b/data/CF.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E61F17-5C48-4FE1-9751-59291F71512F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E7EC05B6-B8E5-4AA4-8741-F13D16ABA8C6}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="9" firstSheet="4" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="EmailLocationCampaign" sheetId="1" r:id="rId1"/>
-    <sheet name="EmailBrandCampaign" sheetId="6" r:id="rId2"/>
-    <sheet name="EmailMultiLocation" sheetId="8" r:id="rId3"/>
-    <sheet name="GRLocationCampaign" sheetId="5" r:id="rId4"/>
-    <sheet name="GRLBrandCampaign" sheetId="7" r:id="rId5"/>
-    <sheet name="GRLMultiLocation" sheetId="9" r:id="rId6"/>
-    <sheet name="Date" sheetId="2" r:id="rId7"/>
-    <sheet name="Reschedule Date" sheetId="3" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId9"/>
-    <sheet name="Filters" sheetId="10" r:id="rId10"/>
+    <sheet name="EmailLocationCampaign" r:id="rId1" sheetId="1"/>
+    <sheet name="EmailBrandCampaign" r:id="rId2" sheetId="6"/>
+    <sheet name="EmailMultiLocation" r:id="rId3" sheetId="8"/>
+    <sheet name="GRLocationCampaign" r:id="rId4" sheetId="5"/>
+    <sheet name="GRLBrandCampaign" r:id="rId5" sheetId="7"/>
+    <sheet name="GRLMultiLocation" r:id="rId6" sheetId="9"/>
+    <sheet name="Date" r:id="rId7" sheetId="2"/>
+    <sheet name="Reschedule Date" r:id="rId8" sheetId="3"/>
+    <sheet name="Sheet1" r:id="rId9" sheetId="4"/>
+    <sheet name="Filters" r:id="rId10" sheetId="10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="80">
   <si>
     <t>CamType</t>
   </si>
@@ -268,13 +268,20 @@
     <t>FilterSetUp</t>
   </si>
   <si>
-    <t>null</t>
+    <t>Select setup</t>
+  </si>
+  <si>
+    <t>Camp Name</t>
+  </si>
+  <si>
+    <t>Bug 110617 Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -318,39 +325,39 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -367,10 +374,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -405,7 +412,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -440,7 +447,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -534,21 +541,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -565,7 +572,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -617,15 +624,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
@@ -633,22 +640,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="79" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -710,7 +717,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -771,28 +778,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{6384C7A0-8601-4AE5-BE16-86FB9C21A5D1}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7CE0A5-DECB-4987-BD51-DB8EFDE59B69}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7CE0A5-DECB-4987-BD51-DB8EFDE59B69}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>75</v>
       </c>
@@ -800,15 +808,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -816,7 +827,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -824,7 +835,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -833,13 +844,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180802A0-94AE-4CA7-8363-1BACCC04771F}">
-  <dimension ref="A1:X2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{180802A0-94AE-4CA7-8363-1BACCC04771F}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:Q2"/>
@@ -847,34 +859,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="38.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="81.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="39.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="34.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="11.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="11.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="23.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="38.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="14.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="81.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="34.28515625" collapsed="true"/>
+    <col min="25" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -948,7 +960,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1022,16 +1034,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{EFD0683B-08D1-422F-95F9-F3247753FAE0}"/>
+    <hyperlink r:id="rId1" ref="L2" xr:uid="{EFD0683B-08D1-422F-95F9-F3247753FAE0}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B2BB62-79BB-4A73-9996-95362A466A26}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B2BB62-79BB-4A73-9996-95362A466A26}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection sqref="A1:J2"/>
@@ -1039,25 +1051,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="81.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="39.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="38.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="27" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="32.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="81.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="24.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="23.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="38.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="27.0" collapsed="true"/>
+    <col min="16" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1152,14 +1164,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEEBA94E-5E2C-4F6D-8E38-1335CE7FDF6B}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:I2"/>
@@ -1167,16 +1179,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1241,31 +1253,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62030C4F-85F5-4D7C-AEBE-444ECD7E4204}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62030C4F-85F5-4D7C-AEBE-444ECD7E4204}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="10" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="8" max="10" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1363,14 +1375,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F67BC90-6774-475B-9753-7D297B7B4830}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F67BC90-6774-475B-9753-7D297B7B4830}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
@@ -1378,16 +1390,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="81.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1455,13 +1467,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9587D94-9F03-4DF5-81BD-372303C1378E}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1532,13 +1544,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5442F-6603-432F-ACFF-AFB1279FFC3B}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -1609,13 +1621,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368A9EC-3397-40E7-82FE-40F00D6168CF}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1627,6 +1639,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>